<commit_message>
Fixed a bug where not all references would be inputted into the database
To be fair: this bug isn't fixed. It was intentional.
Documents that do not have DOIs labelled as: {10.XYZ} (WITH THE FIRST THREE CHARACTERS BEING EXACTLY "10.") are not added to the list of references. Because of this, the arraylist of SLRs could read

Article 1
Article 3
Article 4
Article 5

If article 2 had an improperly formatted doi. This is intentional for the time being but is important to note. There is now a println that displays if an article has an improperly formatted doi, though it is still not added to the list of references.
</commit_message>
<xml_diff>
--- a/Covid_19_Dataset_and_References/References/31.xlsx
+++ b/Covid_19_Dataset_and_References/References/31.xlsx
@@ -1,19 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\CovidClef2023\covidClef2023\Covid_19_Dataset_and_References\References\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B0B197-36C3-40AE-A980-33DC6741FE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="11115" yWindow="1545" windowWidth="17250" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>Doi</t>
   </si>
@@ -36,9 +43,6 @@
     <t>10.1007/s00330-020-06829-2</t>
   </si>
   <si>
-    <t>doi.org/10.1148/radiol.2020201237</t>
-  </si>
-  <si>
     <t>10.1007/s11604-020-00958-w</t>
   </si>
   <si>
@@ -69,28 +73,19 @@
     <t>Authors</t>
   </si>
   <si>
-    <t>Unknown Title</t>
-  </si>
-  <si>
-    <t>Unknown Abstract</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
     <t>ID Format</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>not found</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Date Accepted</t>
+  </si>
+  <si>
+    <t>10.1148/radiol.2020201237</t>
+  </si>
+  <si>
+    <t>Other found locations</t>
   </si>
   <si>
     <t>Correlation of Chest CT and RT-PCR Testing in Coronavirus Disease 2019 (COVID-19) in China: A Report of 1014 Cases</t>
@@ -116,7 +111,7 @@
 </t>
   </si>
   <si>
-    <t>[Tao%Ai%NULL%1, Zhenlu%Yang%NULL%2, Zhenlu%Yang%NULL%0, Hongyan%Hou%NULL%2, Hongyan%Hou%NULL%0, Chenao%Zhan%NULL%1, Chong%Chen%NULL%1, Wenzhi%Lv%NULL%2, Wenzhi%Lv%NULL%0, Qian%Tao%NULL%2, Qian%Tao%NULL%0, Ziyong%Sun%NULL%2, Ziyong%Sun%NULL%0, Liming%Xia%xialiming2017@outlook.com%1]</t>
+    <t>[Tao%Ai%NULL%0, Zhenlu%Yang%NULL%2, Zhenlu%Yang%NULL%0, Hongyan%Hou%NULL%2, Hongyan%Hou%NULL%0, Chenao%Zhan%NULL%1, Chong%Chen%NULL%1, Wenzhi%Lv%NULL%2, Wenzhi%Lv%NULL%0, Qian%Tao%NULL%2, Qian%Tao%NULL%0, Ziyong%Sun%NULL%2, Ziyong%Sun%NULL%0, Liming%Xia%xialiming2017@outlook.com%1]</t>
   </si>
   <si>
     <t>PMC7233399</t>
@@ -126,6 +121,9 @@
   </si>
   <si>
     <t>1970-01-01</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Performance of radiologists in differentiating COVID-19 from viral pneumonia on chest CT</t>
@@ -166,6 +164,21 @@
     <t>PMC7233414</t>
   </si>
   <si>
+    <t>Unknown Title</t>
+  </si>
+  <si>
+    <t>Unknown Abstract</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>Extension of Coronavirus Disease 2019 on Chest CT and Implications for Chest Radiographic Interpretation</t>
   </si>
   <si>
@@ -238,6 +251,40 @@
     <t>2020-03-23</t>
   </si>
   <si>
+    <t>_Springer</t>
+  </si>
+  <si>
+    <t>Chest CT Features of COVID-19 in Rome, Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background
+The standard for diagnosis of SARS-CoV-2 virus is reverse transcription polymerase chain reaction (RT-PCR) test, but chest CT may play a complimentary role in the early detection of COVID-19 pneumonia.
+Purpose
+To investigate CT features of patients with COVID-19 in Rome, Italy, and to compare the accuracy of CT with RT-PCR.
+Methods
+In this prospective study from March 4, 2020, until March 19, 2020, consecutive patients with suspected COVID-19 infection and respiratory symptoms were enrolled.
+ Exclusion criteria were: chest CT with contrast medium performed for vascular indications, patients who refused chest CT or hospitalization, and severe CT motion artifact.
+ All patients underwent RT-PCR and chest CT.
+ Diagnostic performance of CT was calculated using RT-PCR as reference.
+ Chest CT features were calculated in a subgroup of RT-PCR-positive and CT-positive patients.
+ CT features of hospitalized patients and patient in home isolation were compared by using Pearson chi squared test.
+Results
+Our study population comprised 158 consecutive study participants (83 male and 75 female, mean age 57 y ±17).
+ Fever was observed in 97/158 (61%), cough in 88/158 (56%), dyspnea in 52/158 (33%), lymphocytopenia in 95/158 (60%), increased C-reactive protein level in 139/158 (88%), and elevated lactate dehydrogenase in 128/158 (81%) study participants.
+ Sensitivity, specificity, and accuracy of CT were 97% (60/62)[95% IC, 88-99%], 56% (54/96)[95% IC,45-66%] and 72% (114/158)[95% IC 64-78%], respectively.
+ In the subgroup of RT-PCR-positive and CT-positive patients, ground-glass opacities (GGO) were present in 58/58 (100%), multilobe and posterior involvement were both present in 54/58 (93%), bilateral pneumonia in 53/58 (91%), and subsegmental vessel enlargement (&amp;gt; 3 mm) in 52/58 (89%) of study participants.
+Conclusion
+The typical pattern of COVID-19 pneumonia in Rome, Italy, was peripherally ground-glass opacities with multilobe and posterior involvement, bilateral distribution, and subsegmental vessel enlargement (&amp;gt; 3 mm).
+ Chest CT sensitivity was high (97%) but with lower specificity (56%).
+</t>
+  </si>
+  <si>
+    <t>[Damiano%Caruso%NULL%0, Marta%Zerunian%NULL%2, Marta%Zerunian%NULL%0, Michela%Polici%NULL%2, Michela%Polici%NULL%0, Francesco%Pucciarelli%NULL%2, Francesco%Pucciarelli%NULL%0, Tiziano%Polidori%NULL%2, Tiziano%Polidori%NULL%0, Carlotta%Rucci%NULL%2, Carlotta%Rucci%NULL%0, Gisella%Guido%NULL%2, Gisella%Guido%NULL%0, Benedetta%Bracci%NULL%2, Benedetta%Bracci%NULL%0, Chiara%de Dominicis%NULL%2, Chiara%de Dominicis%NULL%0, Andrea%Laghi%andrea.laghi@uniroma1.it%2, Andrea%Laghi%andrea.laghi@uniroma1.it%0]</t>
+  </si>
+  <si>
+    <t>PMC7194020</t>
+  </si>
+  <si>
     <t>Diagnostic performance of chest CT to differentiate COVID-19 pneumonia in non-high-epidemic area in Japan</t>
   </si>
   <si>
@@ -280,6 +327,9 @@
   </si>
   <si>
     <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>_elsevier</t>
   </si>
   <si>
     <t>Early chest computed tomography to diagnose COVID-19 from suspected patients: A multicenter retrospective study</t>
@@ -305,7 +355,7 @@
 </t>
   </si>
   <si>
-    <t>[Congliang%Miao%NULL%1, Mengdi%Jin%NULL%1, Li%Miao%NULL%1, Xinying%Yang%NULL%1, Peng%Huang%NULL%1, Huanwen%Xiong%NULL%1, Peijie%Huang%NULL%1, Qi%Zhao%NULL%1, Jiang%Du%NULL%1, Jiang%Hong%NULL%1]</t>
+    <t>[Congliang%Miao%NULL%1, Mengdi%Jin%NULL%1, Li%Miao%NULL%1, Xinying%Yang%NULL%1, Peng%Huang%NULL%1, Huanwen%Xiong%NULL%1, Peijie%Huang%NULL%1, Qi%Zhao%NULL%1, Jiang%Du%NULL%0, Jiang%Hong%NULL%1]</t>
   </si>
   <si>
     <t>PMC7166306</t>
@@ -336,7 +386,7 @@
 </t>
   </si>
   <si>
-    <t>[Zeying%Wen%NULL%1, Yonge%Chi%NULL%2, Yonge%Chi%NULL%0, Liang%Zhang%NULL%2, Liang%Zhang%NULL%0, Huan%Liu%NULL%2, Huan%Liu%NULL%0, Kun%Du%NULL%1, Zhengxing%Li%NULL%2, Zhengxing%Li%NULL%0, Jie%Chen%NULL%2, Jie%Chen%NULL%0, Liuhui%Cheng%NULL%2, Liuhui%Cheng%NULL%0, Daoqing%Wang%wangdaoqing1215@126.com%2, Daoqing%Wang%wangdaoqing1215@126.com%0]</t>
+    <t>[Zeying%Wen%NULL%1, Yonge%Chi%NULL%2, Yonge%Chi%NULL%0, Liang%Zhang%NULL%2, Liang%Zhang%NULL%0, Huan%Liu%NULL%2, Huan%Liu%NULL%0, Kun%Du%NULL%1, Zhengxing%Li%NULL%2, Zhengxing%Li%NULL%0, Jie%Chen%NULL%0, Jie%Chen%NULL%0, Liuhui%Cheng%NULL%2, Liuhui%Cheng%NULL%0, Daoqing%Wang%wangdaoqing1215@126.com%2, Daoqing%Wang%wangdaoqing1215@126.com%0]</t>
   </si>
   <si>
     <t>PMC7194021</t>
@@ -451,39 +501,43 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="mmm d yyyy"/>
-    <numFmt numFmtId="165" formatCode="mmmm d, yyyy"/>
-    <numFmt numFmtId="166" formatCode="d mmmm yyyy"/>
-    <numFmt numFmtId="167" formatCode="mmmm yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\ d\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="d\ mmmm\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -491,7 +545,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -507,62 +561,56 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -752,20 +800,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,357 +826,417 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>43887.0</v>
+        <v>43887</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>43900.0</v>
+        <v>43900</v>
       </c>
       <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>43888</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5">
-        <v>43888.0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>27</v>
+      </c>
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>43920.0</v>
+        <v>43920</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
-        <v>43937.0</v>
+      <c r="B6" s="6">
+        <v>43937</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>47</v>
+      </c>
+      <c r="I6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43924</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
-        <v>43924.0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B8" s="6">
+        <v>43920</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7">
-        <v>43920.0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="8" t="s">
+      <c r="B9" s="8">
+        <v>43952</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="9">
-        <v>43952.0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="8">
+        <v>44348</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="9">
-        <v>44348.0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B11" s="3">
+        <v>43927</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <v>44013</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3">
-        <v>43927.0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="9">
-        <v>44013.0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="10">
+        <v>43903</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="11">
-        <v>43903.0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="B14" s="3">
-        <v>43942.0</v>
+        <v>43942</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
-    <hyperlink r:id="rId3" ref="A5"/>
-    <hyperlink r:id="rId4" ref="A7"/>
-    <hyperlink r:id="rId5" ref="A9"/>
-    <hyperlink r:id="rId6" ref="A10"/>
-    <hyperlink r:id="rId7" ref="A11"/>
-    <hyperlink r:id="rId8" ref="A12"/>
-    <hyperlink r:id="rId9" ref="A13"/>
-    <hyperlink r:id="rId10" ref="A14"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A7" r:id="rId4" display="doi.org/10.1148/radiol.2020201237" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>